<commit_message>
aded rf & rfr
</commit_message>
<xml_diff>
--- a/KubeTuner/kubetune1.0/src/models/randomforest/output/kubetune_recommended_cpurequest.xlsx
+++ b/KubeTuner/kubetune1.0/src/models/randomforest/output/kubetune_recommended_cpurequest.xlsx
@@ -530,10 +530,10 @@
         <v>0.008999999999999999</v>
       </c>
       <c r="D5" t="n">
-        <v>0.008999999999999999</v>
+        <v>0.01</v>
       </c>
       <c r="E5" t="n">
-        <v>0.011</v>
+        <v>0.012</v>
       </c>
     </row>
     <row r="6">
@@ -644,10 +644,10 @@
         <v>0.048</v>
       </c>
       <c r="D11" t="n">
-        <v>0.048</v>
+        <v>0.049</v>
       </c>
       <c r="E11" t="n">
-        <v>0.058</v>
+        <v>0.059</v>
       </c>
     </row>
     <row r="12">
@@ -796,7 +796,7 @@
         <v>0.056</v>
       </c>
       <c r="D19" t="n">
-        <v>0.056</v>
+        <v>0.055</v>
       </c>
       <c r="E19" t="n">
         <v>0.067</v>
@@ -853,7 +853,7 @@
         <v>0.049</v>
       </c>
       <c r="D22" t="n">
-        <v>0.049</v>
+        <v>0.048</v>
       </c>
       <c r="E22" t="n">
         <v>0.059</v>
@@ -1214,10 +1214,10 @@
         <v>0.008</v>
       </c>
       <c r="D41" t="n">
-        <v>0.008</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="E41" t="n">
-        <v>0.01</v>
+        <v>0.011</v>
       </c>
     </row>
     <row r="42">
@@ -1309,7 +1309,7 @@
         <v>0.015</v>
       </c>
       <c r="D46" t="n">
-        <v>0.015</v>
+        <v>0.014</v>
       </c>
       <c r="E46" t="n">
         <v>0.018</v>
@@ -1480,7 +1480,7 @@
         <v>0.022</v>
       </c>
       <c r="D55" t="n">
-        <v>0.022</v>
+        <v>0.021</v>
       </c>
       <c r="E55" t="n">
         <v>0.026</v>
@@ -3171,7 +3171,7 @@
         <v>0.039</v>
       </c>
       <c r="D144" t="n">
-        <v>0.039</v>
+        <v>0.038</v>
       </c>
       <c r="E144" t="n">
         <v>0.047</v>
@@ -3361,10 +3361,10 @@
         <v>0.048</v>
       </c>
       <c r="D154" t="n">
-        <v>0.048</v>
+        <v>0.049</v>
       </c>
       <c r="E154" t="n">
-        <v>0.058</v>
+        <v>0.059</v>
       </c>
     </row>
     <row r="155">
@@ -3513,7 +3513,7 @@
         <v>0.056</v>
       </c>
       <c r="D162" t="n">
-        <v>0.056</v>
+        <v>0.055</v>
       </c>
       <c r="E162" t="n">
         <v>0.067</v>
@@ -3551,10 +3551,10 @@
         <v>0.053</v>
       </c>
       <c r="D164" t="n">
-        <v>0.053</v>
+        <v>0.054</v>
       </c>
       <c r="E164" t="n">
-        <v>0.064</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="165">
@@ -3570,7 +3570,7 @@
         <v>0.049</v>
       </c>
       <c r="D165" t="n">
-        <v>0.049</v>
+        <v>0.048</v>
       </c>
       <c r="E165" t="n">
         <v>0.059</v>
@@ -3931,10 +3931,10 @@
         <v>0.008</v>
       </c>
       <c r="D184" t="n">
-        <v>0.008</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="E184" t="n">
-        <v>0.01</v>
+        <v>0.011</v>
       </c>
     </row>
     <row r="185">
@@ -4026,7 +4026,7 @@
         <v>0.015</v>
       </c>
       <c r="D189" t="n">
-        <v>0.015</v>
+        <v>0.014</v>
       </c>
       <c r="E189" t="n">
         <v>0.018</v>
@@ -4102,7 +4102,7 @@
         <v>53.006</v>
       </c>
       <c r="D193" t="n">
-        <v>53.006</v>
+        <v>40.185</v>
       </c>
       <c r="E193" t="n">
         <v>63.607</v>
@@ -4121,7 +4121,7 @@
         <v>37.722</v>
       </c>
       <c r="D194" t="n">
-        <v>37.722</v>
+        <v>34.835</v>
       </c>
       <c r="E194" t="n">
         <v>45.266</v>
@@ -4235,7 +4235,7 @@
         <v>0.022</v>
       </c>
       <c r="D200" t="n">
-        <v>0.022</v>
+        <v>0.021</v>
       </c>
       <c r="E200" t="n">
         <v>0.026</v>
@@ -6116,10 +6116,10 @@
         <v>0.048</v>
       </c>
       <c r="D299" t="n">
-        <v>0.048</v>
+        <v>0.049</v>
       </c>
       <c r="E299" t="n">
-        <v>0.058</v>
+        <v>0.059</v>
       </c>
     </row>
     <row r="300">
@@ -6154,7 +6154,7 @@
         <v>0.066</v>
       </c>
       <c r="D301" t="n">
-        <v>0.066</v>
+        <v>0.059</v>
       </c>
       <c r="E301" t="n">
         <v>0.079</v>
@@ -6268,7 +6268,7 @@
         <v>0.056</v>
       </c>
       <c r="D307" t="n">
-        <v>0.056</v>
+        <v>0.055</v>
       </c>
       <c r="E307" t="n">
         <v>0.067</v>
@@ -6306,10 +6306,10 @@
         <v>0.054</v>
       </c>
       <c r="D309" t="n">
-        <v>0.054</v>
+        <v>0.055</v>
       </c>
       <c r="E309" t="n">
-        <v>0.065</v>
+        <v>0.066</v>
       </c>
     </row>
     <row r="310">
@@ -6325,7 +6325,7 @@
         <v>0.049</v>
       </c>
       <c r="D310" t="n">
-        <v>0.049</v>
+        <v>0.048</v>
       </c>
       <c r="E310" t="n">
         <v>0.059</v>
@@ -6686,10 +6686,10 @@
         <v>0.008</v>
       </c>
       <c r="D329" t="n">
-        <v>0.008</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="E329" t="n">
-        <v>0.01</v>
+        <v>0.011</v>
       </c>
     </row>
     <row r="330">
@@ -6781,7 +6781,7 @@
         <v>0.015</v>
       </c>
       <c r="D334" t="n">
-        <v>0.015</v>
+        <v>0.014</v>
       </c>
       <c r="E334" t="n">
         <v>0.018</v>
@@ -6952,7 +6952,7 @@
         <v>0.022</v>
       </c>
       <c r="D343" t="n">
-        <v>0.022</v>
+        <v>0.021</v>
       </c>
       <c r="E343" t="n">
         <v>0.026</v>
@@ -8833,10 +8833,10 @@
         <v>0.048</v>
       </c>
       <c r="D442" t="n">
-        <v>0.048</v>
+        <v>0.049</v>
       </c>
       <c r="E442" t="n">
-        <v>0.058</v>
+        <v>0.059</v>
       </c>
     </row>
     <row r="443">
@@ -8871,7 +8871,7 @@
         <v>0.066</v>
       </c>
       <c r="D444" t="n">
-        <v>0.066</v>
+        <v>0.059</v>
       </c>
       <c r="E444" t="n">
         <v>0.079</v>
@@ -8985,7 +8985,7 @@
         <v>0.056</v>
       </c>
       <c r="D450" t="n">
-        <v>0.056</v>
+        <v>0.055</v>
       </c>
       <c r="E450" t="n">
         <v>0.067</v>
@@ -9023,10 +9023,10 @@
         <v>0.054</v>
       </c>
       <c r="D452" t="n">
-        <v>0.054</v>
+        <v>0.055</v>
       </c>
       <c r="E452" t="n">
-        <v>0.065</v>
+        <v>0.066</v>
       </c>
     </row>
     <row r="453">
@@ -9042,7 +9042,7 @@
         <v>0.049</v>
       </c>
       <c r="D453" t="n">
-        <v>0.049</v>
+        <v>0.048</v>
       </c>
       <c r="E453" t="n">
         <v>0.059</v>
@@ -9403,10 +9403,10 @@
         <v>0.008</v>
       </c>
       <c r="D472" t="n">
-        <v>0.008</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="E472" t="n">
-        <v>0.01</v>
+        <v>0.011</v>
       </c>
     </row>
     <row r="473">
@@ -9498,7 +9498,7 @@
         <v>0.015</v>
       </c>
       <c r="D477" t="n">
-        <v>0.015</v>
+        <v>0.014</v>
       </c>
       <c r="E477" t="n">
         <v>0.018</v>
@@ -9669,7 +9669,7 @@
         <v>0.022</v>
       </c>
       <c r="D486" t="n">
-        <v>0.022</v>
+        <v>0.021</v>
       </c>
       <c r="E486" t="n">
         <v>0.026</v>
@@ -11531,10 +11531,10 @@
         <v>0.048</v>
       </c>
       <c r="D584" t="n">
-        <v>0.048</v>
+        <v>0.049</v>
       </c>
       <c r="E584" t="n">
-        <v>0.058</v>
+        <v>0.059</v>
       </c>
     </row>
     <row r="585">
@@ -11683,7 +11683,7 @@
         <v>0.056</v>
       </c>
       <c r="D592" t="n">
-        <v>0.056</v>
+        <v>0.055</v>
       </c>
       <c r="E592" t="n">
         <v>0.067</v>
@@ -11721,10 +11721,10 @@
         <v>0.053</v>
       </c>
       <c r="D594" t="n">
-        <v>0.053</v>
+        <v>0.054</v>
       </c>
       <c r="E594" t="n">
-        <v>0.064</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="595">
@@ -11740,7 +11740,7 @@
         <v>0.049</v>
       </c>
       <c r="D595" t="n">
-        <v>0.049</v>
+        <v>0.048</v>
       </c>
       <c r="E595" t="n">
         <v>0.059</v>
@@ -12101,10 +12101,10 @@
         <v>0.008</v>
       </c>
       <c r="D614" t="n">
-        <v>0.008</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="E614" t="n">
-        <v>0.01</v>
+        <v>0.011</v>
       </c>
     </row>
     <row r="615">
@@ -12196,7 +12196,7 @@
         <v>0.015</v>
       </c>
       <c r="D619" t="n">
-        <v>0.015</v>
+        <v>0.014</v>
       </c>
       <c r="E619" t="n">
         <v>0.018</v>
@@ -12367,7 +12367,7 @@
         <v>0.022</v>
       </c>
       <c r="D628" t="n">
-        <v>0.022</v>
+        <v>0.021</v>
       </c>
       <c r="E628" t="n">
         <v>0.026</v>
@@ -14248,10 +14248,10 @@
         <v>0.048</v>
       </c>
       <c r="D727" t="n">
-        <v>0.048</v>
+        <v>0.049</v>
       </c>
       <c r="E727" t="n">
-        <v>0.058</v>
+        <v>0.059</v>
       </c>
     </row>
     <row r="728">
@@ -14400,7 +14400,7 @@
         <v>0.056</v>
       </c>
       <c r="D735" t="n">
-        <v>0.056</v>
+        <v>0.055</v>
       </c>
       <c r="E735" t="n">
         <v>0.067</v>
@@ -14438,10 +14438,10 @@
         <v>0.053</v>
       </c>
       <c r="D737" t="n">
-        <v>0.053</v>
+        <v>0.054</v>
       </c>
       <c r="E737" t="n">
-        <v>0.064</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="738">
@@ -14457,7 +14457,7 @@
         <v>0.049</v>
       </c>
       <c r="D738" t="n">
-        <v>0.049</v>
+        <v>0.048</v>
       </c>
       <c r="E738" t="n">
         <v>0.059</v>
@@ -14818,10 +14818,10 @@
         <v>0.008</v>
       </c>
       <c r="D757" t="n">
-        <v>0.008</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="E757" t="n">
-        <v>0.01</v>
+        <v>0.011</v>
       </c>
     </row>
     <row r="758">
@@ -14913,7 +14913,7 @@
         <v>0.015</v>
       </c>
       <c r="D762" t="n">
-        <v>0.015</v>
+        <v>0.014</v>
       </c>
       <c r="E762" t="n">
         <v>0.018</v>
@@ -15084,7 +15084,7 @@
         <v>0.022</v>
       </c>
       <c r="D771" t="n">
-        <v>0.022</v>
+        <v>0.021</v>
       </c>
       <c r="E771" t="n">
         <v>0.026</v>
@@ -16965,10 +16965,10 @@
         <v>0.048</v>
       </c>
       <c r="D870" t="n">
-        <v>0.048</v>
+        <v>0.049</v>
       </c>
       <c r="E870" t="n">
-        <v>0.058</v>
+        <v>0.059</v>
       </c>
     </row>
     <row r="871">
@@ -17117,7 +17117,7 @@
         <v>0.056</v>
       </c>
       <c r="D878" t="n">
-        <v>0.056</v>
+        <v>0.055</v>
       </c>
       <c r="E878" t="n">
         <v>0.067</v>
@@ -17155,10 +17155,10 @@
         <v>0.053</v>
       </c>
       <c r="D880" t="n">
-        <v>0.053</v>
+        <v>0.054</v>
       </c>
       <c r="E880" t="n">
-        <v>0.064</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="881">
@@ -17174,7 +17174,7 @@
         <v>0.049</v>
       </c>
       <c r="D881" t="n">
-        <v>0.049</v>
+        <v>0.048</v>
       </c>
       <c r="E881" t="n">
         <v>0.059</v>
@@ -17535,10 +17535,10 @@
         <v>0.008</v>
       </c>
       <c r="D900" t="n">
-        <v>0.008</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="E900" t="n">
-        <v>0.01</v>
+        <v>0.011</v>
       </c>
     </row>
     <row r="901">
@@ -17630,7 +17630,7 @@
         <v>0.015</v>
       </c>
       <c r="D905" t="n">
-        <v>0.015</v>
+        <v>0.014</v>
       </c>
       <c r="E905" t="n">
         <v>0.018</v>
@@ -17801,7 +17801,7 @@
         <v>0.022</v>
       </c>
       <c r="D914" t="n">
-        <v>0.022</v>
+        <v>0.021</v>
       </c>
       <c r="E914" t="n">
         <v>0.026</v>

</xml_diff>